<commit_message>
Updated dats with SLR thoughts
</commit_message>
<xml_diff>
--- a/resources/Dates_W20A.xlsx
+++ b/resources/Dates_W20A.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>url</t>
   </si>
@@ -83,9 +83,6 @@
     <t>ANOVA1 -- Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">SLR -- </t>
-  </si>
-  <si>
     <t xml:space="preserve">IVR -- </t>
   </si>
   <si>
@@ -147,6 +144,42 @@
   </si>
   <si>
     <t>ANOVA2Summary</t>
+  </si>
+  <si>
+    <t>SLR -- Foundations</t>
+  </si>
+  <si>
+    <t>SLR -- Inference</t>
+  </si>
+  <si>
+    <t>SLR -- Models</t>
+  </si>
+  <si>
+    <t>SLR -- Assumptions</t>
+  </si>
+  <si>
+    <t>SLR -- Summary</t>
+  </si>
+  <si>
+    <t>SLR -- Transformations</t>
+  </si>
+  <si>
+    <t>SLRFoundations</t>
+  </si>
+  <si>
+    <t>SLRInference</t>
+  </si>
+  <si>
+    <t>SLRModels</t>
+  </si>
+  <si>
+    <t>SLRAssumptions</t>
+  </si>
+  <si>
+    <t>SLRTransformations</t>
+  </si>
+  <si>
+    <t>SLRSummary</t>
   </si>
 </sst>
 </file>
@@ -531,7 +564,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +619,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -604,7 +637,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -622,7 +655,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -640,7 +673,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -655,10 +688,10 @@
         <v>44223</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -676,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -712,7 +745,7 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -730,7 +763,7 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -745,10 +778,10 @@
         <v>44230</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -763,10 +796,10 @@
         <v>44231</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,10 +814,10 @@
         <v>44232</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -799,10 +832,10 @@
         <v>44235</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -817,10 +850,13 @@
         <v>44236</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -832,10 +868,13 @@
         <v>44237</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -847,10 +886,13 @@
         <v>44238</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -862,10 +904,13 @@
         <v>44239</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -877,10 +922,13 @@
         <v>44242</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -892,10 +940,13 @@
         <v>44243</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -907,10 +958,10 @@
         <v>44244</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -922,10 +973,10 @@
         <v>44245</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -937,10 +988,10 @@
         <v>44246</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -952,10 +1003,10 @@
         <v>44249</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -967,10 +1018,10 @@
         <v>44250</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -982,10 +1033,10 @@
         <v>44251</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -997,10 +1048,10 @@
         <v>44252</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1012,10 +1063,10 @@
         <v>44253</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -1027,10 +1078,10 @@
         <v>44256</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -1042,10 +1093,10 @@
         <v>44257</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -1057,7 +1108,7 @@
         <v>44258</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1072,7 +1123,7 @@
         <v>44259</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1087,7 +1138,7 @@
         <v>44260</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>